<commit_message>
Implement team statistics calculation and sorting in standings renderer
</commit_message>
<xml_diff>
--- a/templates/league_data.xlsx
+++ b/templates/league_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leejt\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leejt\OneDrive\Documents\GitHub\nbcml\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4632C966-892A-4D5D-BB88-709D59653AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A047AF-525B-4F06-A7A5-0B9B2E799F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
@@ -1048,7 +1048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B089AB-C826-4619-B243-5B13AFD7DC37}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2642,7 +2642,7 @@
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30:U32"/>
+      <selection activeCell="E7" sqref="E7:U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3015,9 +3015,15 @@
       <c r="D7" t="s">
         <v>4</v>
       </c>
+      <c r="E7">
+        <v>49</v>
+      </c>
       <c r="F7" t="s">
         <v>60</v>
       </c>
+      <c r="G7">
+        <v>53</v>
+      </c>
       <c r="H7" t="s">
         <v>18</v>
       </c>
@@ -3027,9 +3033,15 @@
       <c r="J7" t="s">
         <v>61</v>
       </c>
+      <c r="K7">
+        <v>58</v>
+      </c>
       <c r="L7" t="s">
         <v>34</v>
       </c>
+      <c r="M7">
+        <v>67</v>
+      </c>
       <c r="N7" t="s">
         <v>72</v>
       </c>
@@ -3039,8 +3051,14 @@
       <c r="P7" t="s">
         <v>62</v>
       </c>
+      <c r="Q7">
+        <v>80</v>
+      </c>
       <c r="R7" t="s">
         <v>59</v>
+      </c>
+      <c r="S7">
+        <v>100</v>
       </c>
       <c r="T7" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Update league data Excel template and remove temporary file
</commit_message>
<xml_diff>
--- a/templates/league_data.xlsx
+++ b/templates/league_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leejt\OneDrive\Documents\GitHub\nbcml\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A047AF-525B-4F06-A7A5-0B9B2E799F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="rosters" sheetId="1" r:id="rId1"/>
@@ -1048,7 +1048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B089AB-C826-4619-B243-5B13AFD7DC37}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2641,7 +2641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA593B-70CA-4B35-A8AE-58F429AF5E66}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7:U7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Refactor pre-season rendering logic to use async data fetching and improve error handling; add new pre-season CSV data file
</commit_message>
<xml_diff>
--- a/templates/league_data.xlsx
+++ b/templates/league_data.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leejt\OneDrive\Documents\GitHub\nbcml\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4C6AA22-4D47-4ADD-B118-A30D56791D73}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10060" activeTab="2" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="rosters" sheetId="1" r:id="rId1"/>
-    <sheet name="games" sheetId="2" r:id="rId2"/>
+    <sheet name="regseason" sheetId="2" r:id="rId2"/>
+    <sheet name="preseason" sheetId="3" r:id="rId3"/>
+    <sheet name="playoffs" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="293">
   <si>
     <t>Team</t>
   </si>
@@ -667,6 +669,255 @@
   </si>
   <si>
     <t>12-23-2025</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Robinson</t>
+  </si>
+  <si>
+    <t>Wright</t>
+  </si>
+  <si>
+    <t>Murphy</t>
+  </si>
+  <si>
+    <t>Collins</t>
+  </si>
+  <si>
+    <t>Edwards</t>
+  </si>
+  <si>
+    <t>Phillips</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>Butler</t>
+  </si>
+  <si>
+    <t>Turner</t>
+  </si>
+  <si>
+    <t>Ross</t>
+  </si>
+  <si>
+    <t>Coleman</t>
+  </si>
+  <si>
+    <t>Hill</t>
+  </si>
+  <si>
+    <t>Baker</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Young</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Mitchell</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Adams</t>
+  </si>
+  <si>
+    <t>Hall</t>
+  </si>
+  <si>
+    <t>Nelson</t>
+  </si>
+  <si>
+    <t>Torres</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>Ward</t>
+  </si>
+  <si>
+    <t>Watson</t>
+  </si>
+  <si>
+    <t>Brooks</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Bennett</t>
+  </si>
+  <si>
+    <t>Hughes</t>
+  </si>
+  <si>
+    <t>Cox</t>
+  </si>
+  <si>
+    <t>Bailey</t>
+  </si>
+  <si>
+    <t>Richardson</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>Kenneth</t>
+  </si>
+  <si>
+    <t>Ronald</t>
+  </si>
+  <si>
+    <t>Timothy</t>
+  </si>
+  <si>
+    <t>Gary</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Jeffrey</t>
+  </si>
+  <si>
+    <t>Larry</t>
+  </si>
+  <si>
+    <t>Donald</t>
+  </si>
+  <si>
+    <t>Gregory</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>Jerry</t>
+  </si>
+  <si>
+    <t>Carl</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Albert</t>
+  </si>
+  <si>
+    <t>Wayne</t>
+  </si>
+  <si>
+    <t>Bruce</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Vincent</t>
+  </si>
+  <si>
+    <t>Todd</t>
   </si>
 </sst>
 </file>
@@ -708,10 +959,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1048,7 +1301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B089AB-C826-4619-B243-5B13AFD7DC37}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2642,7 +2895,7 @@
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:U7"/>
+      <selection activeCell="E7" sqref="A1:U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4207,4 +4460,1034 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACA149D-F9A7-48BD-BB53-827DF1410F23}">
+  <dimension ref="A1:F49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" customWidth="1"/>
+    <col min="7" max="7" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="7.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E10" t="s">
+        <v>197</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>264</v>
+      </c>
+      <c r="C11" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C12" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E12" t="s">
+        <v>197</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" t="s">
+        <v>219</v>
+      </c>
+      <c r="D13" t="s">
+        <v>196</v>
+      </c>
+      <c r="E13" t="s">
+        <v>197</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>267</v>
+      </c>
+      <c r="C14" t="s">
+        <v>220</v>
+      </c>
+      <c r="D14" t="s">
+        <v>196</v>
+      </c>
+      <c r="E14" t="s">
+        <v>197</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>268</v>
+      </c>
+      <c r="C15" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15" t="s">
+        <v>196</v>
+      </c>
+      <c r="E15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>222</v>
+      </c>
+      <c r="D16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E16" t="s">
+        <v>197</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>223</v>
+      </c>
+      <c r="D17" t="s">
+        <v>196</v>
+      </c>
+      <c r="E17" t="s">
+        <v>197</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D18" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" t="s">
+        <v>197</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>225</v>
+      </c>
+      <c r="D19" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>269</v>
+      </c>
+      <c r="C20" t="s">
+        <v>226</v>
+      </c>
+      <c r="D20" t="s">
+        <v>196</v>
+      </c>
+      <c r="E20" t="s">
+        <v>197</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>270</v>
+      </c>
+      <c r="C21" t="s">
+        <v>227</v>
+      </c>
+      <c r="D21" t="s">
+        <v>196</v>
+      </c>
+      <c r="E21" t="s">
+        <v>197</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>228</v>
+      </c>
+      <c r="D22" t="s">
+        <v>196</v>
+      </c>
+      <c r="E22" t="s">
+        <v>197</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>271</v>
+      </c>
+      <c r="C23" t="s">
+        <v>229</v>
+      </c>
+      <c r="D23" t="s">
+        <v>196</v>
+      </c>
+      <c r="E23" t="s">
+        <v>197</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>272</v>
+      </c>
+      <c r="C24" t="s">
+        <v>230</v>
+      </c>
+      <c r="D24" t="s">
+        <v>196</v>
+      </c>
+      <c r="E24" t="s">
+        <v>197</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>273</v>
+      </c>
+      <c r="C25" t="s">
+        <v>231</v>
+      </c>
+      <c r="D25" t="s">
+        <v>196</v>
+      </c>
+      <c r="E25" t="s">
+        <v>197</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="4">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>274</v>
+      </c>
+      <c r="C26" t="s">
+        <v>232</v>
+      </c>
+      <c r="D26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" t="s">
+        <v>197</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>275</v>
+      </c>
+      <c r="C27" t="s">
+        <v>233</v>
+      </c>
+      <c r="D27" t="s">
+        <v>196</v>
+      </c>
+      <c r="E27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>276</v>
+      </c>
+      <c r="C28" t="s">
+        <v>234</v>
+      </c>
+      <c r="D28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E28" t="s">
+        <v>197</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="4">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>277</v>
+      </c>
+      <c r="C29" t="s">
+        <v>235</v>
+      </c>
+      <c r="D29" t="s">
+        <v>196</v>
+      </c>
+      <c r="E29" t="s">
+        <v>197</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="4">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s">
+        <v>236</v>
+      </c>
+      <c r="D30" t="s">
+        <v>196</v>
+      </c>
+      <c r="E30" t="s">
+        <v>197</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="4">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" t="s">
+        <v>237</v>
+      </c>
+      <c r="D31" t="s">
+        <v>196</v>
+      </c>
+      <c r="E31" t="s">
+        <v>197</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="4">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>278</v>
+      </c>
+      <c r="C32" t="s">
+        <v>238</v>
+      </c>
+      <c r="D32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E32" t="s">
+        <v>197</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="4">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>279</v>
+      </c>
+      <c r="C33" t="s">
+        <v>239</v>
+      </c>
+      <c r="D33" t="s">
+        <v>196</v>
+      </c>
+      <c r="E33" t="s">
+        <v>197</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="4">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>280</v>
+      </c>
+      <c r="C34" t="s">
+        <v>240</v>
+      </c>
+      <c r="D34" t="s">
+        <v>196</v>
+      </c>
+      <c r="E34" t="s">
+        <v>197</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="4">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>281</v>
+      </c>
+      <c r="C35" t="s">
+        <v>241</v>
+      </c>
+      <c r="D35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E35" t="s">
+        <v>197</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="4">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>282</v>
+      </c>
+      <c r="C36" t="s">
+        <v>242</v>
+      </c>
+      <c r="D36" t="s">
+        <v>196</v>
+      </c>
+      <c r="E36" t="s">
+        <v>197</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="4">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>283</v>
+      </c>
+      <c r="C37" t="s">
+        <v>243</v>
+      </c>
+      <c r="D37" t="s">
+        <v>196</v>
+      </c>
+      <c r="E37" t="s">
+        <v>197</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="4">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>284</v>
+      </c>
+      <c r="C38" t="s">
+        <v>244</v>
+      </c>
+      <c r="D38" t="s">
+        <v>196</v>
+      </c>
+      <c r="E38" t="s">
+        <v>197</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="4">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s">
+        <v>245</v>
+      </c>
+      <c r="D39" t="s">
+        <v>196</v>
+      </c>
+      <c r="E39" t="s">
+        <v>197</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="4">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>285</v>
+      </c>
+      <c r="C40" t="s">
+        <v>246</v>
+      </c>
+      <c r="D40" t="s">
+        <v>196</v>
+      </c>
+      <c r="E40" t="s">
+        <v>197</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="4">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" t="s">
+        <v>247</v>
+      </c>
+      <c r="D41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E41" t="s">
+        <v>197</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="4">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>286</v>
+      </c>
+      <c r="C42" t="s">
+        <v>248</v>
+      </c>
+      <c r="D42" t="s">
+        <v>196</v>
+      </c>
+      <c r="E42" t="s">
+        <v>197</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="4">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>287</v>
+      </c>
+      <c r="C43" t="s">
+        <v>249</v>
+      </c>
+      <c r="D43" t="s">
+        <v>196</v>
+      </c>
+      <c r="E43" t="s">
+        <v>197</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="4">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>288</v>
+      </c>
+      <c r="C44" t="s">
+        <v>250</v>
+      </c>
+      <c r="D44" t="s">
+        <v>196</v>
+      </c>
+      <c r="E44" t="s">
+        <v>197</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="4">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>289</v>
+      </c>
+      <c r="C45" t="s">
+        <v>251</v>
+      </c>
+      <c r="D45" t="s">
+        <v>196</v>
+      </c>
+      <c r="E45" t="s">
+        <v>197</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="4">
+        <v>3</v>
+      </c>
+      <c r="B46" t="s">
+        <v>290</v>
+      </c>
+      <c r="C46" t="s">
+        <v>252</v>
+      </c>
+      <c r="D46" t="s">
+        <v>196</v>
+      </c>
+      <c r="E46" t="s">
+        <v>197</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="4">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>291</v>
+      </c>
+      <c r="C47" t="s">
+        <v>253</v>
+      </c>
+      <c r="D47" t="s">
+        <v>196</v>
+      </c>
+      <c r="E47" t="s">
+        <v>197</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="4">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" t="s">
+        <v>254</v>
+      </c>
+      <c r="D48" t="s">
+        <v>196</v>
+      </c>
+      <c r="E48" t="s">
+        <v>197</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="4">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>292</v>
+      </c>
+      <c r="C49" t="s">
+        <v>255</v>
+      </c>
+      <c r="D49" t="s">
+        <v>196</v>
+      </c>
+      <c r="E49" t="s">
+        <v>197</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031C8247-C053-4190-8C4D-407C16576311}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: update league_data.xlsx to reflect recent changes
</commit_message>
<xml_diff>
--- a/templates/league_data.xlsx
+++ b/templates/league_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4C6AA22-4D47-4ADD-B118-A30D56791D73}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C743231D-E6DB-418A-9BC5-9E9EB58AAB15}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10060" activeTab="2" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" activeTab="1" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="rosters" sheetId="1" r:id="rId1"/>
@@ -2894,8 +2894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA593B-70CA-4B35-A8AE-58F429AF5E66}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="A1:U35"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3333,9 +3333,15 @@
       <c r="D8" t="s">
         <v>34</v>
       </c>
+      <c r="E8">
+        <v>682</v>
+      </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
+      <c r="G8">
+        <v>82</v>
+      </c>
       <c r="H8" t="s">
         <v>20</v>
       </c>
@@ -3345,9 +3351,15 @@
       <c r="J8" t="s">
         <v>60</v>
       </c>
+      <c r="K8">
+        <v>76</v>
+      </c>
       <c r="L8" t="s">
         <v>59</v>
       </c>
+      <c r="M8">
+        <v>70</v>
+      </c>
       <c r="N8" t="s">
         <v>74</v>
       </c>
@@ -3357,8 +3369,14 @@
       <c r="P8" t="s">
         <v>61</v>
       </c>
+      <c r="Q8">
+        <v>50</v>
+      </c>
       <c r="R8" t="s">
         <v>4</v>
+      </c>
+      <c r="S8">
+        <v>70</v>
       </c>
       <c r="T8" t="s">
         <v>53</v>
@@ -4466,7 +4484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACA149D-F9A7-48BD-BB53-827DF1410F23}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix: update scores for Week 7 in regseason.csv and refresh league_data.xlsx
</commit_message>
<xml_diff>
--- a/templates/league_data.xlsx
+++ b/templates/league_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C743231D-E6DB-418A-9BC5-9E9EB58AAB15}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{751BFFD0-9B7E-4D3D-89B0-2B4273CBEFDC}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" activeTab="1" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="rosters" sheetId="1" r:id="rId1"/>
@@ -2894,8 +2894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA593B-70CA-4B35-A8AE-58F429AF5E66}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3334,7 +3334,7 @@
         <v>34</v>
       </c>
       <c r="E8">
-        <v>682</v>
+        <v>82</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
feat: enhance schedule loading with debug logging and improve CSS for special cells
</commit_message>
<xml_diff>
--- a/templates/league_data.xlsx
+++ b/templates/league_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{751BFFD0-9B7E-4D3D-89B0-2B4273CBEFDC}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1C2714D-0349-4212-A73B-3A9A2491D04C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="rosters" sheetId="1" r:id="rId1"/>
     <sheet name="regseason" sheetId="2" r:id="rId2"/>
     <sheet name="preseason" sheetId="3" r:id="rId3"/>
     <sheet name="playoffs" sheetId="4" r:id="rId4"/>
+    <sheet name="champs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="315">
   <si>
     <t>Team</t>
   </si>
@@ -918,6 +919,72 @@
   </si>
   <si>
     <t>Todd</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>p6</t>
+  </si>
+  <si>
+    <t>p7</t>
+  </si>
+  <si>
+    <t>p8</t>
+  </si>
+  <si>
+    <t>p9</t>
+  </si>
+  <si>
+    <t>Frank Vucko</t>
+  </si>
+  <si>
+    <t>James Wang</t>
+  </si>
+  <si>
+    <t>Mav Marick</t>
+  </si>
+  <si>
+    <t>George Sparangis</t>
+  </si>
+  <si>
+    <t>Petar Rafajlovic</t>
+  </si>
+  <si>
+    <t>Ralph Romano</t>
+  </si>
+  <si>
+    <t>Richard Montoya</t>
+  </si>
+  <si>
+    <t>Sean Ludwig</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>Magna Centre</t>
+  </si>
+  <si>
+    <t>Sacred Heart</t>
   </si>
 </sst>
 </file>
@@ -2894,29 +2961,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA593B-70CA-4B35-A8AE-58F429AF5E66}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.36328125" customWidth="1"/>
+    <col min="2" max="2" width="4.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.6328125" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="12.54296875" customWidth="1"/>
+    <col min="14" max="14" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.26953125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="7.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
@@ -5500,12 +5570,444 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031C8247-C053-4190-8C4D-407C16576311}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="7.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N1" t="s">
+        <v>203</v>
+      </c>
+      <c r="O1" t="s">
+        <v>204</v>
+      </c>
+      <c r="P1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>162</v>
+      </c>
+      <c r="R1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S1" t="s">
+        <v>164</v>
+      </c>
+      <c r="T1" t="s">
+        <v>205</v>
+      </c>
+      <c r="U1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4805BFD7-430C-410D-A776-3D2E58164FD3}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G1" t="s">
+        <v>298</v>
+      </c>
+      <c r="H1" t="s">
+        <v>299</v>
+      </c>
+      <c r="I1" t="s">
+        <v>300</v>
+      </c>
+      <c r="J1" t="s">
+        <v>301</v>
+      </c>
+      <c r="K1" t="s">
+        <v>302</v>
+      </c>
+      <c r="L1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2025</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G2" t="s">
+        <v>307</v>
+      </c>
+      <c r="H2" t="s">
+        <v>308</v>
+      </c>
+      <c r="I2" t="s">
+        <v>309</v>
+      </c>
+      <c r="J2" t="s">
+        <v>310</v>
+      </c>
+      <c r="K2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2024</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2023</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2021</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2020</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2019</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2018</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2017</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2016</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2015</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2014</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2013</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2012</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2011</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2010</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2009</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2008</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2007</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2006</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>314</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add champs.csv file with historical league data
</commit_message>
<xml_diff>
--- a/templates/league_data.xlsx
+++ b/templates/league_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1C2714D-0349-4212-A73B-3A9A2491D04C}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD2D9966-91D5-4C80-B755-580DEC02E537}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="324">
   <si>
     <t>Team</t>
   </si>
@@ -985,6 +985,33 @@
   </si>
   <si>
     <t>Sacred Heart</t>
+  </si>
+  <si>
+    <t>Mike Johnson</t>
+  </si>
+  <si>
+    <t>Kevin Wilson</t>
+  </si>
+  <si>
+    <t>Paul Taylor</t>
+  </si>
+  <si>
+    <t>Dan Martin</t>
+  </si>
+  <si>
+    <t>Adam Hall</t>
+  </si>
+  <si>
+    <t>Owen Lopez</t>
+  </si>
+  <si>
+    <t>Martin Paul</t>
+  </si>
+  <si>
+    <t>Jim Beam</t>
+  </si>
+  <si>
+    <t>Phil McCrakin</t>
   </si>
 </sst>
 </file>
@@ -5706,7 +5733,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4805BFD7-430C-410D-A776-3D2E58164FD3}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:L3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -5721,7 +5750,7 @@
     <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -5807,6 +5836,33 @@
       <c r="C3" t="s">
         <v>313</v>
       </c>
+      <c r="D3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E3" t="s">
+        <v>316</v>
+      </c>
+      <c r="F3" t="s">
+        <v>317</v>
+      </c>
+      <c r="G3" t="s">
+        <v>318</v>
+      </c>
+      <c r="H3" t="s">
+        <v>319</v>
+      </c>
+      <c r="I3" t="s">
+        <v>320</v>
+      </c>
+      <c r="J3" t="s">
+        <v>321</v>
+      </c>
+      <c r="K3" t="s">
+        <v>322</v>
+      </c>
+      <c r="L3" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">

</xml_diff>

<commit_message>
feat: update league_data.xlsx with new league statistics
</commit_message>
<xml_diff>
--- a/templates/league_data.xlsx
+++ b/templates/league_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD2D9966-91D5-4C80-B755-580DEC02E537}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E014B85F-570E-4D6F-A106-0951CC6D4087}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="324">
   <si>
     <t>Team</t>
   </si>
@@ -5731,10 +5731,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4805BFD7-430C-410D-A776-3D2E58164FD3}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:L3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5742,7 +5742,7 @@
     <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
@@ -5949,7 +5949,7 @@
         <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
@@ -5960,7 +5960,7 @@
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -5971,7 +5971,7 @@
         <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -5982,7 +5982,7 @@
         <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -5993,7 +5993,7 @@
         <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -6004,7 +6004,7 @@
         <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -6015,7 +6015,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -6026,7 +6026,7 @@
         <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -6037,7 +6037,7 @@
         <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -6048,7 +6048,7 @@
         <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -6062,8 +6062,108 @@
         <v>314</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2005</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2004</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2003</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2002</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2001</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2000</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>1999</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>1998</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>1997</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>314</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update regseason.csv with missing scores and correct league_data.xlsx
</commit_message>
<xml_diff>
--- a/templates/league_data.xlsx
+++ b/templates/league_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E014B85F-570E-4D6F-A106-0951CC6D4087}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{EC426CBF-EB95-40B7-8A45-6C5D9E5FCC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFC524EB-10AD-4945-B045-AD7A7B566A25}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="rosters" sheetId="1" r:id="rId1"/>
@@ -2988,8 +2988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA593B-70CA-4B35-A8AE-58F429AF5E66}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3495,9 +3495,15 @@
       <c r="D9" t="s">
         <v>61</v>
       </c>
+      <c r="E9">
+        <v>35</v>
+      </c>
       <c r="F9" t="s">
         <v>59</v>
       </c>
+      <c r="G9">
+        <v>37</v>
+      </c>
       <c r="H9" t="s">
         <v>22</v>
       </c>
@@ -3507,9 +3513,15 @@
       <c r="J9" t="s">
         <v>4</v>
       </c>
+      <c r="K9">
+        <v>67</v>
+      </c>
       <c r="L9" t="s">
         <v>62</v>
       </c>
+      <c r="M9">
+        <v>55</v>
+      </c>
       <c r="N9" t="s">
         <v>9</v>
       </c>
@@ -3519,8 +3531,14 @@
       <c r="P9" t="s">
         <v>60</v>
       </c>
+      <c r="Q9">
+        <v>58</v>
+      </c>
       <c r="R9" t="s">
         <v>34</v>
+      </c>
+      <c r="S9">
+        <v>56</v>
       </c>
       <c r="T9" t="s">
         <v>55</v>
@@ -3542,9 +3560,15 @@
       <c r="D10" t="s">
         <v>59</v>
       </c>
+      <c r="E10">
+        <v>77</v>
+      </c>
       <c r="F10" t="s">
         <v>34</v>
       </c>
+      <c r="G10">
+        <v>69</v>
+      </c>
       <c r="H10" t="s">
         <v>24</v>
       </c>
@@ -3554,9 +3578,15 @@
       <c r="J10" t="s">
         <v>62</v>
       </c>
+      <c r="K10">
+        <v>105</v>
+      </c>
       <c r="L10" t="s">
         <v>61</v>
       </c>
+      <c r="M10">
+        <v>101</v>
+      </c>
       <c r="N10" t="s">
         <v>77</v>
       </c>
@@ -3566,8 +3596,14 @@
       <c r="P10" t="s">
         <v>4</v>
       </c>
+      <c r="Q10">
+        <v>53</v>
+      </c>
       <c r="R10" t="s">
         <v>60</v>
+      </c>
+      <c r="S10">
+        <v>50</v>
       </c>
       <c r="T10" t="s">
         <v>57</v>
@@ -5733,7 +5769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4805BFD7-430C-410D-A776-3D2E58164FD3}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>

</xml_diff>